<commit_message>
some direct solution script; a pdf for config
</commit_message>
<xml_diff>
--- a/UploadData/extract/uploadExtracts_fromCSV_TEMPLATE.xlsx
+++ b/UploadData/extract/uploadExtracts_fromCSV_TEMPLATE.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pierrespc/Documents/PostDocPasteur/aDNA/Import_eLAB/API_FUNCTIONALITIES/UploadData/extract/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82849EE8-90C1-3745-8EA7-545C008384D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8300D6B0-1DD1-9846-B88F-65931BB9F602}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="780" yWindow="1000" windowWidth="27640" windowHeight="16180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1152,17 +1152,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:V17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="V2" sqref="V2"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="22.1640625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="17.5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="17" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="19" max="19" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="17.1640625" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="13.83203125" bestFit="1" customWidth="1"/>

</xml_diff>